<commit_message>
C30 - Update WebApiWithAspDotNet6.xlsx
</commit_message>
<xml_diff>
--- a/WebApiWithAspDotNet6.xlsx
+++ b/WebApiWithAspDotNet6.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Chung" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Chung!$A$1:$AC$559</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Chung!$A$1:$AC$565</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="101">
   <si>
     <t>ASP.NET CORE API WEB APP (&gt;&lt;)</t>
   </si>
@@ -375,7 +375,7 @@
     <t>JSON Web Tokens (JWT)</t>
   </si>
   <si>
-    <t>Microsoft.AspNetCore.Authentication.JwtBearer</t>
+    <t>Microsoft.AspNetCore.Authentication.JwtBearer (6.0.15)</t>
   </si>
   <si>
     <t>Microsoft.IdentityModel.Tokens</t>
@@ -384,10 +384,22 @@
     <t>System.IdentityModel.Tokens.Jwt</t>
   </si>
   <si>
-    <t>1. Create TokenHandler class (Repository)</t>
+    <t>1. Create TokenHandler class (Service)</t>
   </si>
   <si>
     <t>2. AuthController (using TokenHandler)</t>
+  </si>
+  <si>
+    <t>3. Add authentication to services</t>
+  </si>
+  <si>
+    <t>4. Jwt constant information</t>
+  </si>
+  <si>
+    <t>12.</t>
+  </si>
+  <si>
+    <t>Logger</t>
   </si>
 </sst>
 </file>
@@ -395,10 +407,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -463,6 +475,20 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -478,15 +504,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -495,90 +515,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -594,7 +530,69 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -602,6 +600,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -652,7 +664,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,31 +826,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -700,139 +838,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -937,6 +949,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -952,17 +979,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1000,28 +1023,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1037,13 +1049,13 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1055,130 +1067,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1372,8 +1384,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>87</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -1393,7 +1405,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="497840" y="13060680"/>
-          <a:ext cx="5943600" cy="2705100"/>
+          <a:ext cx="5946775" cy="2705100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4364,8 +4376,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>311785</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>186</xdr:row>
       <xdr:rowOff>48895</xdr:rowOff>
     </xdr:to>
@@ -4385,7 +4397,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="496570" y="29615130"/>
-          <a:ext cx="5942330" cy="3554095"/>
+          <a:ext cx="5948045" cy="3554095"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5602,8 +5614,8 @@
       <xdr:rowOff>128270</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>309245</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>398</xdr:row>
       <xdr:rowOff>36830</xdr:rowOff>
     </xdr:to>
@@ -5623,7 +5635,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="496570" y="68331080"/>
-          <a:ext cx="3082290" cy="2362200"/>
+          <a:ext cx="3090545" cy="2362200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7593,6 +7605,690 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>517</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>136525</xdr:colOff>
+      <xdr:row>530</xdr:row>
+      <xdr:rowOff>125095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="497840" y="91718130"/>
+          <a:ext cx="6718300" cy="2403475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>117475</xdr:colOff>
+      <xdr:row>519</xdr:row>
+      <xdr:rowOff>40005</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>521</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="Oval 67"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5927090" y="92108655"/>
+          <a:ext cx="320675" cy="326390"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>2</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>307975</xdr:colOff>
+      <xdr:row>533</xdr:row>
+      <xdr:rowOff>52705</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>146685</xdr:colOff>
+      <xdr:row>541</xdr:row>
+      <xdr:rowOff>64135</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="74" name="Picture 73"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="488315" y="94574995"/>
+          <a:ext cx="6737985" cy="1413510"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>116840</xdr:colOff>
+      <xdr:row>535</xdr:row>
+      <xdr:rowOff>128270</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>120015</xdr:colOff>
+      <xdr:row>537</xdr:row>
+      <xdr:rowOff>104140</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="75" name="Oval 74"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5926455" y="95001080"/>
+          <a:ext cx="320675" cy="326390"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>3</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>307340</xdr:colOff>
+      <xdr:row>541</xdr:row>
+      <xdr:rowOff>125095</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>545</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="76" name="Picture 75"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="487680" y="96049465"/>
+          <a:ext cx="5761355" cy="667385"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>136525</xdr:colOff>
+      <xdr:row>543</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>545</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="77" name="Oval 76"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4041140" y="96324420"/>
+          <a:ext cx="320675" cy="326390"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>3</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>307340</xdr:colOff>
+      <xdr:row>548</xdr:row>
+      <xdr:rowOff>46355</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>97790</xdr:colOff>
+      <xdr:row>554</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="78" name="Picture 77"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="487680" y="97197545"/>
+          <a:ext cx="4149725" cy="1176655"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7881,9 +8577,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:AB558"/>
+  <dimension ref="B1:AB564"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -23581,7 +24277,9 @@
     </row>
     <row r="533" spans="2:28">
       <c r="B533" s="10"/>
-      <c r="C533" s="11"/>
+      <c r="C533" s="22" t="s">
+        <v>97</v>
+      </c>
       <c r="D533" s="13"/>
       <c r="E533" s="12"/>
       <c r="F533" s="12"/>
@@ -24016,7 +24714,9 @@
     </row>
     <row r="548" spans="2:28">
       <c r="B548" s="10"/>
-      <c r="C548" s="11"/>
+      <c r="C548" s="22" t="s">
+        <v>98</v>
+      </c>
       <c r="D548" s="13"/>
       <c r="E548" s="12"/>
       <c r="F548" s="12"/>
@@ -24275,63 +24975,241 @@
       <c r="AA556" s="12"/>
       <c r="AB556" s="19"/>
     </row>
-    <row r="557" spans="2:28">
-      <c r="B557" s="10"/>
-      <c r="C557" s="11"/>
-      <c r="D557" s="13"/>
-      <c r="E557" s="12"/>
-      <c r="F557" s="12"/>
-      <c r="G557" s="12"/>
-      <c r="H557" s="12"/>
-      <c r="I557" s="12"/>
-      <c r="J557" s="12"/>
-      <c r="K557" s="12"/>
-      <c r="L557" s="12"/>
-      <c r="M557" s="12"/>
-      <c r="N557" s="12"/>
-      <c r="O557" s="12"/>
-      <c r="P557" s="12"/>
-      <c r="Q557" s="12"/>
-      <c r="R557" s="12"/>
-      <c r="S557" s="12"/>
-      <c r="T557" s="12"/>
-      <c r="U557" s="12"/>
-      <c r="V557" s="12"/>
-      <c r="W557" s="12"/>
-      <c r="X557" s="12"/>
-      <c r="Y557" s="12"/>
-      <c r="Z557" s="12"/>
-      <c r="AA557" s="12"/>
-      <c r="AB557" s="19"/>
-    </row>
-    <row r="558" ht="14.55" spans="2:28">
-      <c r="B558" s="29"/>
-      <c r="C558" s="30"/>
-      <c r="D558" s="31"/>
-      <c r="E558" s="31"/>
-      <c r="F558" s="31"/>
-      <c r="G558" s="31"/>
-      <c r="H558" s="31"/>
-      <c r="I558" s="31"/>
-      <c r="J558" s="31"/>
-      <c r="K558" s="31"/>
-      <c r="L558" s="31"/>
-      <c r="M558" s="31"/>
-      <c r="N558" s="31"/>
-      <c r="O558" s="31"/>
-      <c r="P558" s="31"/>
-      <c r="Q558" s="31"/>
-      <c r="R558" s="31"/>
-      <c r="S558" s="31"/>
-      <c r="T558" s="31"/>
-      <c r="U558" s="31"/>
-      <c r="V558" s="31"/>
-      <c r="W558" s="31"/>
-      <c r="X558" s="31"/>
-      <c r="Y558" s="31"/>
-      <c r="Z558" s="31"/>
-      <c r="AA558" s="31"/>
-      <c r="AB558" s="32"/>
+    <row r="557" ht="20.1" customHeight="1" spans="2:28">
+      <c r="B557" s="8"/>
+      <c r="C557" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D557" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E557" s="9"/>
+      <c r="F557" s="9"/>
+      <c r="G557" s="9"/>
+      <c r="H557" s="9"/>
+      <c r="I557" s="9"/>
+      <c r="J557" s="9"/>
+      <c r="K557" s="9"/>
+      <c r="L557" s="9"/>
+      <c r="M557" s="9"/>
+      <c r="N557" s="9"/>
+      <c r="O557" s="9"/>
+      <c r="P557" s="9"/>
+      <c r="Q557" s="9"/>
+      <c r="R557" s="9"/>
+      <c r="S557" s="9"/>
+      <c r="T557" s="9"/>
+      <c r="U557" s="9"/>
+      <c r="V557" s="9"/>
+      <c r="W557" s="9"/>
+      <c r="X557" s="9"/>
+      <c r="Y557" s="9"/>
+      <c r="Z557" s="9"/>
+      <c r="AA557" s="9"/>
+      <c r="AB557" s="18"/>
+    </row>
+    <row r="558" spans="2:28">
+      <c r="B558" s="10"/>
+      <c r="C558" s="11"/>
+      <c r="D558" s="13"/>
+      <c r="E558" s="12"/>
+      <c r="F558" s="12"/>
+      <c r="G558" s="12"/>
+      <c r="H558" s="12"/>
+      <c r="I558" s="12"/>
+      <c r="J558" s="12"/>
+      <c r="K558" s="12"/>
+      <c r="L558" s="12"/>
+      <c r="M558" s="12"/>
+      <c r="N558" s="12"/>
+      <c r="O558" s="12"/>
+      <c r="P558" s="12"/>
+      <c r="Q558" s="12"/>
+      <c r="R558" s="12"/>
+      <c r="S558" s="12"/>
+      <c r="T558" s="12"/>
+      <c r="U558" s="12"/>
+      <c r="V558" s="12"/>
+      <c r="W558" s="12"/>
+      <c r="X558" s="12"/>
+      <c r="Y558" s="12"/>
+      <c r="Z558" s="12"/>
+      <c r="AA558" s="12"/>
+      <c r="AB558" s="19"/>
+    </row>
+    <row r="559" spans="2:28">
+      <c r="B559" s="10"/>
+      <c r="C559" s="11"/>
+      <c r="D559" s="13"/>
+      <c r="E559" s="12"/>
+      <c r="F559" s="12"/>
+      <c r="G559" s="12"/>
+      <c r="H559" s="12"/>
+      <c r="I559" s="12"/>
+      <c r="J559" s="12"/>
+      <c r="K559" s="12"/>
+      <c r="L559" s="12"/>
+      <c r="M559" s="12"/>
+      <c r="N559" s="12"/>
+      <c r="O559" s="12"/>
+      <c r="P559" s="12"/>
+      <c r="Q559" s="12"/>
+      <c r="R559" s="12"/>
+      <c r="S559" s="12"/>
+      <c r="T559" s="12"/>
+      <c r="U559" s="12"/>
+      <c r="V559" s="12"/>
+      <c r="W559" s="12"/>
+      <c r="X559" s="12"/>
+      <c r="Y559" s="12"/>
+      <c r="Z559" s="12"/>
+      <c r="AA559" s="12"/>
+      <c r="AB559" s="19"/>
+    </row>
+    <row r="560" spans="2:28">
+      <c r="B560" s="10"/>
+      <c r="C560" s="11"/>
+      <c r="D560" s="13"/>
+      <c r="E560" s="12"/>
+      <c r="F560" s="12"/>
+      <c r="G560" s="12"/>
+      <c r="H560" s="12"/>
+      <c r="I560" s="12"/>
+      <c r="J560" s="12"/>
+      <c r="K560" s="12"/>
+      <c r="L560" s="12"/>
+      <c r="M560" s="12"/>
+      <c r="N560" s="12"/>
+      <c r="O560" s="12"/>
+      <c r="P560" s="12"/>
+      <c r="Q560" s="12"/>
+      <c r="R560" s="12"/>
+      <c r="S560" s="12"/>
+      <c r="T560" s="12"/>
+      <c r="U560" s="12"/>
+      <c r="V560" s="12"/>
+      <c r="W560" s="12"/>
+      <c r="X560" s="12"/>
+      <c r="Y560" s="12"/>
+      <c r="Z560" s="12"/>
+      <c r="AA560" s="12"/>
+      <c r="AB560" s="19"/>
+    </row>
+    <row r="561" spans="2:28">
+      <c r="B561" s="10"/>
+      <c r="C561" s="11"/>
+      <c r="D561" s="13"/>
+      <c r="E561" s="12"/>
+      <c r="F561" s="12"/>
+      <c r="G561" s="12"/>
+      <c r="H561" s="12"/>
+      <c r="I561" s="12"/>
+      <c r="J561" s="12"/>
+      <c r="K561" s="12"/>
+      <c r="L561" s="12"/>
+      <c r="M561" s="12"/>
+      <c r="N561" s="12"/>
+      <c r="O561" s="12"/>
+      <c r="P561" s="12"/>
+      <c r="Q561" s="12"/>
+      <c r="R561" s="12"/>
+      <c r="S561" s="12"/>
+      <c r="T561" s="12"/>
+      <c r="U561" s="12"/>
+      <c r="V561" s="12"/>
+      <c r="W561" s="12"/>
+      <c r="X561" s="12"/>
+      <c r="Y561" s="12"/>
+      <c r="Z561" s="12"/>
+      <c r="AA561" s="12"/>
+      <c r="AB561" s="19"/>
+    </row>
+    <row r="562" spans="2:28">
+      <c r="B562" s="10"/>
+      <c r="C562" s="11"/>
+      <c r="D562" s="13"/>
+      <c r="E562" s="12"/>
+      <c r="F562" s="12"/>
+      <c r="G562" s="12"/>
+      <c r="H562" s="12"/>
+      <c r="I562" s="12"/>
+      <c r="J562" s="12"/>
+      <c r="K562" s="12"/>
+      <c r="L562" s="12"/>
+      <c r="M562" s="12"/>
+      <c r="N562" s="12"/>
+      <c r="O562" s="12"/>
+      <c r="P562" s="12"/>
+      <c r="Q562" s="12"/>
+      <c r="R562" s="12"/>
+      <c r="S562" s="12"/>
+      <c r="T562" s="12"/>
+      <c r="U562" s="12"/>
+      <c r="V562" s="12"/>
+      <c r="W562" s="12"/>
+      <c r="X562" s="12"/>
+      <c r="Y562" s="12"/>
+      <c r="Z562" s="12"/>
+      <c r="AA562" s="12"/>
+      <c r="AB562" s="19"/>
+    </row>
+    <row r="563" spans="2:28">
+      <c r="B563" s="10"/>
+      <c r="C563" s="11"/>
+      <c r="D563" s="13"/>
+      <c r="E563" s="12"/>
+      <c r="F563" s="12"/>
+      <c r="G563" s="12"/>
+      <c r="H563" s="12"/>
+      <c r="I563" s="12"/>
+      <c r="J563" s="12"/>
+      <c r="K563" s="12"/>
+      <c r="L563" s="12"/>
+      <c r="M563" s="12"/>
+      <c r="N563" s="12"/>
+      <c r="O563" s="12"/>
+      <c r="P563" s="12"/>
+      <c r="Q563" s="12"/>
+      <c r="R563" s="12"/>
+      <c r="S563" s="12"/>
+      <c r="T563" s="12"/>
+      <c r="U563" s="12"/>
+      <c r="V563" s="12"/>
+      <c r="W563" s="12"/>
+      <c r="X563" s="12"/>
+      <c r="Y563" s="12"/>
+      <c r="Z563" s="12"/>
+      <c r="AA563" s="12"/>
+      <c r="AB563" s="19"/>
+    </row>
+    <row r="564" spans="2:28">
+      <c r="B564" s="29"/>
+      <c r="C564" s="30"/>
+      <c r="D564" s="31"/>
+      <c r="E564" s="31"/>
+      <c r="F564" s="31"/>
+      <c r="G564" s="31"/>
+      <c r="H564" s="31"/>
+      <c r="I564" s="31"/>
+      <c r="J564" s="31"/>
+      <c r="K564" s="31"/>
+      <c r="L564" s="31"/>
+      <c r="M564" s="31"/>
+      <c r="N564" s="31"/>
+      <c r="O564" s="31"/>
+      <c r="P564" s="31"/>
+      <c r="Q564" s="31"/>
+      <c r="R564" s="31"/>
+      <c r="S564" s="31"/>
+      <c r="T564" s="31"/>
+      <c r="U564" s="31"/>
+      <c r="V564" s="31"/>
+      <c r="W564" s="31"/>
+      <c r="X564" s="31"/>
+      <c r="Y564" s="31"/>
+      <c r="Z564" s="31"/>
+      <c r="AA564" s="31"/>
+      <c r="AB564" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>